<commit_message>
Ajoute élément manquant pour recherchev
</commit_message>
<xml_diff>
--- a/chiffre affaires.xlsx
+++ b/chiffre affaires.xlsx
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Blue Buffalo</t>
   </si>
   <si>
-    <t xml:space="preserve">USA  </t>
+    <t xml:space="preserve">Chine</t>
   </si>
   <si>
     <t xml:space="preserve">Diamond Pet food</t>
@@ -259,7 +259,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.8"/>
@@ -272,7 +272,7 @@
     <col collapsed="false" hidden="false" max="8" min="7" style="2" width="11.5546558704453"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -305,7 +305,7 @@
       <c r="H3" s="6"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
@@ -326,7 +326,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
@@ -347,7 +347,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
@@ -367,7 +367,7 @@
         <v>9190630.77289839</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
@@ -387,7 +387,7 @@
         <v>14157662.1895968</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
@@ -407,7 +407,7 @@
         <v>164385.703757608</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
@@ -427,7 +427,7 @@
         <v>5768034.74012411</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -447,7 +447,7 @@
         <v>8957076.6789776</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -467,7 +467,7 @@
         <v>13619962.6087798</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -487,7 +487,7 @@
         <v>14159438.2972218</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
@@ -507,7 +507,7 @@
         <v>6091133.61598867</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
@@ -527,7 +527,7 @@
         <v>9226458.49386021</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>27</v>
       </c>
@@ -547,7 +547,7 @@
         <v>12518446.8956049</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
       </c>
@@ -567,7 +567,7 @@
         <v>12386574.5831813</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>30</v>
       </c>
@@ -587,7 +587,7 @@
         <v>45514068.7406715</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -618,7 +618,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5668016194332"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>2</v>
       </c>
@@ -626,7 +626,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -634,7 +634,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -642,7 +642,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -650,7 +650,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>15</v>
       </c>
@@ -658,7 +658,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>17</v>
       </c>
@@ -666,7 +666,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
@@ -674,7 +674,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>24</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>33</v>
       </c>
@@ -690,7 +690,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>31</v>
       </c>

</xml_diff>